<commit_message>
Pettycash api modification , graph y values default to float numbers
</commit_message>
<xml_diff>
--- a/public/pettycashfiles/PC001.xlsx
+++ b/public/pettycashfiles/PC001.xlsx
@@ -11,61 +11,172 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Category code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>DRUVA</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>CARPENTRY</t>
+  </si>
   <si>
     <t>CT</t>
   </si>
   <si>
-    <t>Ply Wood</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Nos</t>
-  </si>
-  <si>
-    <t>{"size":"1800*900","thickness":"6","grade":"MR"}</t>
-  </si>
-  <si>
-    <t>Laminate</t>
-  </si>
-  <si>
-    <t>Merino Lam</t>
-  </si>
-  <si>
-    <t>{"size":"1800 * 1200","thickness":"0.8 mm","grade":"Glossy"}</t>
+    <t>CIVIL &amp; Aggregates</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>ELECTRICAL</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>Electronics &amp; Applicances</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Furnishing Materials</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Furnitures</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>GLASS &amp; MIRROR</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>House Keeping / Cleaning Materials</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Light Fixtures</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Metal &amp; Fabrication Materials</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>Packing Materilas</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PLUMBING</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>POP &amp; Ceiling</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>PPE KIt</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Sanitary &amp; Fixtures</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>Solid Wood</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Stationary</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>stones</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>Tiles</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Tools &amp; Machinery</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>Foam &amp; Sofa Furnising</t>
   </si>
   <si>
     <t>FS</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>{"size":"150mm","thickness":"4 mm","grade":"Heavy"}</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Red Bricks</t>
-  </si>
-  <si>
-    <t>Locally Sourced</t>
-  </si>
-  <si>
-    <t>{"size":"75mm x 100mm x 225mm","thickness":"100 mm"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -73,31 +184,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border/>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -315,7 +470,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="63.25"/>
+    <col customWidth="1" min="1" max="1" width="23.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -328,62 +483,228 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pettycash UI modification with some additional data capture
</commit_message>
<xml_diff>
--- a/public/pettycashfiles/PC001.xlsx
+++ b/public/pettycashfiles/PC001.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,81 +12,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Mobile 1</t>
-  </si>
-  <si>
-    <t>Mobile 2</t>
-  </si>
-  <si>
-    <t>Mobile 3</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Email 1</t>
-  </si>
-  <si>
-    <t>Email 2</t>
-  </si>
-  <si>
-    <t>Email 3</t>
-  </si>
-  <si>
-    <t>TATA CONSUMER SERVICE</t>
-  </si>
-  <si>
-    <t>TATA CHA</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>GST001</t>
-  </si>
-  <si>
-    <t>tata@gmail.com</t>
-  </si>
-  <si>
-    <t>TATA TEA</t>
-  </si>
-  <si>
-    <t>GST003</t>
-  </si>
-  <si>
-    <t>TATA MILK</t>
-  </si>
-  <si>
-    <t>GST004</t>
-  </si>
-  <si>
-    <t>TATA STARBUCKS INDIA PVT LTD</t>
-  </si>
-  <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
-    <t>GST002</t>
-  </si>
-  <si>
-    <t>statbugs@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+  <si>
+    <t>EMPL002</t>
+  </si>
+  <si>
+    <t>Druva Kumar JS</t>
+  </si>
+  <si>
+    <t>druva@gmail.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>druva</t>
+  </si>
+  <si>
+    <t>EMPL003</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>abishek@gmail,com</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>abhishek</t>
+  </si>
+  <si>
+    <t>EMPL004</t>
+  </si>
+  <si>
+    <t>janaki</t>
+  </si>
+  <si>
+    <t>janaki@gmail.com</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>EMPL005</t>
+  </si>
+  <si>
+    <t>shashi</t>
+  </si>
+  <si>
+    <t>shashi@gmail.com</t>
+  </si>
+  <si>
+    <t>procurement</t>
+  </si>
+  <si>
+    <t>EMPL006</t>
+  </si>
+  <si>
+    <t>Susraksah</t>
+  </si>
+  <si>
+    <t>suraksha@gmail.com</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>suraksha</t>
+  </si>
+  <si>
+    <t>EMPL007</t>
+  </si>
+  <si>
+    <t>Kubulu</t>
+  </si>
+  <si>
+    <t>kubulu@gmail.com</t>
+  </si>
+  <si>
+    <t>kubulu</t>
   </si>
 </sst>
 </file>
@@ -100,18 +107,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -123,27 +131,13 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -151,11 +145,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,6 +159,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -372,144 +369,143 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="25.13"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2">
+        <v>8.792422947E9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2">
-        <v>9.63258741E9</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7.89456123E9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9.63258741E9</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
+      <c r="D3" s="2">
+        <v>8.792422946E9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9.63258741E9</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8.792422945E9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.792422944E9</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2">
-        <v>9.632587411E9</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2">
+        <v>8.792422943E9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>